<commit_message>
inclusão de obter estatus do dispositivo
</commit_message>
<xml_diff>
--- a/Doc/ProductBackLogAutomex.xlsx
+++ b/Doc/ProductBackLogAutomex.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Arduino</t>
+  </si>
+  <si>
+    <t>Obter status do dispositivo</t>
   </si>
 </sst>
 </file>
@@ -204,9 +207,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -216,6 +216,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -490,7 +493,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -500,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,19 +540,19 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -595,13 +598,13 @@
         <v>3</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" ref="F5:F50" si="0">E5/D5</f>
+        <f t="shared" ref="F5:F23" si="0">E5/D5</f>
         <v>3</v>
       </c>
       <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="7">
         <v>1</v>
       </c>
     </row>
@@ -628,7 +631,7 @@
       <c r="G6" s="1">
         <v>1</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="7">
         <v>1</v>
       </c>
     </row>
@@ -655,7 +658,7 @@
       <c r="G7" s="1">
         <v>2</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="7">
         <v>1</v>
       </c>
     </row>
@@ -666,7 +669,7 @@
       <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="1">
@@ -682,7 +685,7 @@
       <c r="G8" s="1">
         <v>1</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <v>1</v>
       </c>
     </row>
@@ -693,7 +696,7 @@
       <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="1">
@@ -709,7 +712,7 @@
       <c r="G9" s="1">
         <v>1</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <v>1</v>
       </c>
     </row>
@@ -736,7 +739,7 @@
       <c r="G10" s="2">
         <v>5</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="7">
         <v>0.9</v>
       </c>
       <c r="I10" s="4" t="s">
@@ -766,7 +769,7 @@
       <c r="G11" s="2">
         <v>5</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="7">
         <v>0.9</v>
       </c>
       <c r="I11" s="4" t="s">
@@ -796,7 +799,7 @@
       <c r="G12" s="1">
         <v>1</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="7">
         <v>1</v>
       </c>
     </row>
@@ -823,7 +826,7 @@
       <c r="G13" s="1">
         <v>2</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="7">
         <v>1</v>
       </c>
     </row>
@@ -850,7 +853,7 @@
       <c r="G14" s="1">
         <v>2</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="7">
         <v>1</v>
       </c>
     </row>
@@ -877,7 +880,7 @@
       <c r="G15" s="1">
         <v>2</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="7">
         <v>1</v>
       </c>
     </row>
@@ -904,7 +907,7 @@
       <c r="G16" s="1">
         <v>4</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="7">
         <v>1</v>
       </c>
     </row>
@@ -931,7 +934,7 @@
       <c r="G17" s="1">
         <v>1</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="7">
         <v>1</v>
       </c>
     </row>
@@ -942,13 +945,13 @@
       <c r="B18" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="1">
         <v>8</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="8">
         <v>13</v>
       </c>
       <c r="F18" s="1">
@@ -958,7 +961,7 @@
       <c r="G18" s="2">
         <v>5</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="7">
         <v>0.9</v>
       </c>
       <c r="I18" s="4" t="s">
@@ -988,7 +991,7 @@
       <c r="G19" s="1">
         <v>3</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="7">
         <v>1</v>
       </c>
     </row>
@@ -996,16 +999,16 @@
       <c r="A20" s="4">
         <v>16</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>35</v>
       </c>
       <c r="D20" s="1">
         <v>5</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="8">
         <v>8</v>
       </c>
       <c r="F20" s="1">
@@ -1015,7 +1018,7 @@
       <c r="G20" s="1">
         <v>3</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1023,7 +1026,7 @@
       <c r="A21" s="4">
         <v>17</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1042,7 +1045,7 @@
       <c r="G21" s="1">
         <v>5</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1050,7 +1053,7 @@
       <c r="A22" s="4">
         <v>18</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1069,7 +1072,7 @@
       <c r="G22" s="1">
         <v>1</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H22" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1077,7 +1080,7 @@
       <c r="A23" s="4">
         <v>19</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>34</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -1096,41 +1099,47 @@
       <c r="G23" s="1">
         <v>4</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H24" s="8"/>
+      <c r="A24" s="4">
+        <v>20</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" s="7"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H25" s="8"/>
+      <c r="H25" s="7"/>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H26" s="8"/>
+      <c r="H26" s="7"/>
     </row>
     <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H27" s="8"/>
+      <c r="H27" s="7"/>
     </row>
     <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H28" s="8"/>
+      <c r="H28" s="7"/>
     </row>
     <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H29" s="8"/>
+      <c r="H29" s="7"/>
     </row>
     <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H30" s="8"/>
+      <c r="H30" s="7"/>
     </row>
     <row r="31" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H31" s="8"/>
+      <c r="H31" s="7"/>
     </row>
     <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H32" s="8"/>
+      <c r="H32" s="7"/>
     </row>
     <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H33" s="8"/>
-    </row>
-    <row r="34" spans="1:9" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="1"/>
@@ -1138,37 +1147,37 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="11"/>
+      <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="10"/>
-      <c r="H35" s="8"/>
+      <c r="B35" s="9"/>
+      <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="H36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="12"/>
-      <c r="H37" s="8"/>
+      <c r="B37" s="11"/>
+      <c r="H37" s="7"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H38" s="8"/>
+      <c r="H38" s="7"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H39" s="8"/>
+      <c r="H39" s="7"/>
     </row>
     <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H40" s="8"/>
+      <c r="H40" s="7"/>
     </row>
     <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H41" s="8"/>
+      <c r="H41" s="7"/>
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H42" s="8"/>
-    </row>
-    <row r="43" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H42" s="7"/>
+    </row>
+    <row r="43" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="1"/>
@@ -1176,36 +1185,36 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-      <c r="H43" s="8"/>
+      <c r="H43" s="7"/>
       <c r="I43" s="4"/>
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H44" s="13"/>
+      <c r="H44" s="12"/>
     </row>
     <row r="45" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="10"/>
-      <c r="H45" s="8"/>
+      <c r="B45" s="9"/>
+      <c r="H45" s="7"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H46" s="14"/>
+      <c r="H46" s="13"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H47" s="8"/>
+      <c r="H47" s="7"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H48" s="8"/>
+      <c r="H48" s="7"/>
     </row>
     <row r="49" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H49" s="8"/>
+      <c r="H49" s="7"/>
     </row>
     <row r="50" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H50" s="8"/>
+      <c r="H50" s="7"/>
     </row>
     <row r="51" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H51" s="8"/>
+      <c r="H51" s="7"/>
     </row>
     <row r="53" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H53" s="10"/>
+      <c r="H53" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:I45"/>

</xml_diff>